<commit_message>
Added another way to make a reaction/minspan dict
</commit_message>
<xml_diff>
--- a/data/minspan_EcoliCore.xlsx
+++ b/data/minspan_EcoliCore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38240" windowHeight="20180" tabRatio="764" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19660" tabRatio="764" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2013-11-18_12_59_11" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,184 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="169">
+  <si>
+    <t>ETOHt2r</t>
+  </si>
+  <si>
+    <t>EX_ac(e)</t>
+  </si>
+  <si>
+    <t>EX_acald(e)</t>
+  </si>
+  <si>
+    <t>EX_akg(e)</t>
+  </si>
+  <si>
+    <t>EX_co2(e)</t>
+  </si>
+  <si>
+    <t>EX_etoh(e)</t>
+  </si>
+  <si>
+    <t>EX_for(e)</t>
+  </si>
+  <si>
+    <t>EX_glc(e)</t>
+  </si>
+  <si>
+    <t>EX_glu_L(e)</t>
+  </si>
+  <si>
+    <t>EX_h2o(e)</t>
+  </si>
+  <si>
+    <t>EX_h(e)</t>
+  </si>
+  <si>
+    <t>EX_lac_D(e)</t>
+  </si>
+  <si>
+    <t>EX_nh4(e)</t>
+  </si>
+  <si>
+    <t>EX_o2(e)</t>
+  </si>
+  <si>
+    <t>EX_pyr(e)</t>
+  </si>
+  <si>
+    <t>EX_succ(e)</t>
+  </si>
+  <si>
+    <t>FBA</t>
+  </si>
+  <si>
+    <t>FBP</t>
+  </si>
+  <si>
+    <t>FORt2</t>
+  </si>
+  <si>
+    <t>FORti</t>
+  </si>
+  <si>
+    <t>FRD7</t>
+  </si>
+  <si>
+    <t>FUM</t>
+  </si>
+  <si>
+    <t>G6PDH2r</t>
+  </si>
+  <si>
+    <t>GAPD</t>
+  </si>
+  <si>
+    <t>GLCpts</t>
+  </si>
+  <si>
+    <t>GLNS</t>
+  </si>
+  <si>
+    <t>GLUDy</t>
+  </si>
+  <si>
+    <t>GLUN</t>
+  </si>
+  <si>
+    <t>GLUSy</t>
+  </si>
+  <si>
+    <t>GLUt2r</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>H2Ot</t>
+  </si>
+  <si>
+    <t>ICDHyr</t>
+  </si>
+  <si>
+    <t>ICL</t>
+  </si>
+  <si>
+    <t>LDH_D</t>
+  </si>
+  <si>
+    <t>MALS</t>
+  </si>
+  <si>
+    <t>MDH</t>
+  </si>
+  <si>
+    <t>ME1</t>
+  </si>
+  <si>
+    <t>ME2</t>
+  </si>
+  <si>
+    <t>NADH16</t>
+  </si>
+  <si>
+    <t>NADTRHD</t>
+  </si>
+  <si>
+    <t>NH4t</t>
+  </si>
+  <si>
+    <t>O2t</t>
+  </si>
+  <si>
+    <t>PDH</t>
+  </si>
+  <si>
+    <t>PFK</t>
+  </si>
+  <si>
+    <t>PFL</t>
+  </si>
+  <si>
+    <t>PGI</t>
+  </si>
+  <si>
+    <t>PGK</t>
+  </si>
+  <si>
+    <t>PGL</t>
+  </si>
+  <si>
+    <t>PGM</t>
+  </si>
+  <si>
+    <t>PPC</t>
+  </si>
+  <si>
+    <t>PPCK</t>
+  </si>
+  <si>
+    <t>PPS</t>
+  </si>
+  <si>
+    <t>PTAr</t>
+  </si>
+  <si>
+    <t>PYK</t>
+  </si>
+  <si>
+    <t>PYRt2r</t>
+  </si>
+  <si>
+    <t>RPE</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>SUCCt2_2</t>
+  </si>
   <si>
     <t>EX_h_e</t>
   </si>
@@ -418,183 +595,6 @@
   </si>
   <si>
     <t>ENO</t>
-  </si>
-  <si>
-    <t>ETOHt2r</t>
-  </si>
-  <si>
-    <t>EX_ac(e)</t>
-  </si>
-  <si>
-    <t>EX_acald(e)</t>
-  </si>
-  <si>
-    <t>EX_akg(e)</t>
-  </si>
-  <si>
-    <t>EX_co2(e)</t>
-  </si>
-  <si>
-    <t>EX_etoh(e)</t>
-  </si>
-  <si>
-    <t>EX_for(e)</t>
-  </si>
-  <si>
-    <t>EX_glc(e)</t>
-  </si>
-  <si>
-    <t>EX_glu_L(e)</t>
-  </si>
-  <si>
-    <t>EX_h2o(e)</t>
-  </si>
-  <si>
-    <t>EX_h(e)</t>
-  </si>
-  <si>
-    <t>EX_lac_D(e)</t>
-  </si>
-  <si>
-    <t>EX_nh4(e)</t>
-  </si>
-  <si>
-    <t>EX_o2(e)</t>
-  </si>
-  <si>
-    <t>EX_pyr(e)</t>
-  </si>
-  <si>
-    <t>EX_succ(e)</t>
-  </si>
-  <si>
-    <t>FBA</t>
-  </si>
-  <si>
-    <t>FBP</t>
-  </si>
-  <si>
-    <t>FORt2</t>
-  </si>
-  <si>
-    <t>FORti</t>
-  </si>
-  <si>
-    <t>FRD7</t>
-  </si>
-  <si>
-    <t>FUM</t>
-  </si>
-  <si>
-    <t>G6PDH2r</t>
-  </si>
-  <si>
-    <t>GAPD</t>
-  </si>
-  <si>
-    <t>GLCpts</t>
-  </si>
-  <si>
-    <t>GLNS</t>
-  </si>
-  <si>
-    <t>GLUDy</t>
-  </si>
-  <si>
-    <t>GLUN</t>
-  </si>
-  <si>
-    <t>GLUSy</t>
-  </si>
-  <si>
-    <t>GLUt2r</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>H2Ot</t>
-  </si>
-  <si>
-    <t>ICDHyr</t>
-  </si>
-  <si>
-    <t>ICL</t>
-  </si>
-  <si>
-    <t>LDH_D</t>
-  </si>
-  <si>
-    <t>MALS</t>
-  </si>
-  <si>
-    <t>MDH</t>
-  </si>
-  <si>
-    <t>ME1</t>
-  </si>
-  <si>
-    <t>ME2</t>
-  </si>
-  <si>
-    <t>NADH16</t>
-  </si>
-  <si>
-    <t>NADTRHD</t>
-  </si>
-  <si>
-    <t>NH4t</t>
-  </si>
-  <si>
-    <t>O2t</t>
-  </si>
-  <si>
-    <t>PDH</t>
-  </si>
-  <si>
-    <t>PFK</t>
-  </si>
-  <si>
-    <t>PFL</t>
-  </si>
-  <si>
-    <t>PGI</t>
-  </si>
-  <si>
-    <t>PGK</t>
-  </si>
-  <si>
-    <t>PGL</t>
-  </si>
-  <si>
-    <t>PGM</t>
-  </si>
-  <si>
-    <t>PPC</t>
-  </si>
-  <si>
-    <t>PPCK</t>
-  </si>
-  <si>
-    <t>PPS</t>
-  </si>
-  <si>
-    <t>PTAr</t>
-  </si>
-  <si>
-    <t>PYK</t>
-  </si>
-  <si>
-    <t>PYRt2r</t>
-  </si>
-  <si>
-    <t>RPE</t>
-  </si>
-  <si>
-    <t>RPI</t>
-  </si>
-  <si>
-    <t>SUCCt2_2</t>
   </si>
 </sst>
 </file>
@@ -981,10 +981,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>-6.4427271428077498E-2</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>-1.3245033112582801E-2</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>-1.7094017094017099E-2</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>7.5519581876348002E-3</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="B6">
         <v>7.5519581876348002E-3</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="B7">
         <v>-1.7094017094017099E-2</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B8">
         <v>3.7187359592631399E-2</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B9">
         <v>7.3705546342362296E-4</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="B10">
         <v>-2.92397660818713E-3</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="B11">
         <v>-5.1182238315494802E-2</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="B12">
         <v>0.26919513080620899</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="B13">
         <v>-1.0202927404832401E-2</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B14">
         <v>-2.3225878898450801E-3</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B15">
         <v>7.5519581876348002E-3</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="B16">
         <v>5.2751574799262201E-2</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="B17">
         <v>-0.387382150686086</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="B18">
         <v>0.57033876959477503</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="B19">
         <v>-5.1182238315494802E-2</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>1.7094017094017099E-2</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>1.3245033112582801E-2</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>2.92397660818713E-3</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>2.3225878898450801E-3</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>5.1182238315494802E-2</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>6.6908559955997399E-2</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>-0.285993108026383</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="B27">
         <v>2.8818443804034602E-3</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>0.59935063355959595</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>5.0829542761900701E-2</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>0.387382150686086</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>-2.8818443804034602E-3</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>-2.63757873996311E-2</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>14</v>
       </c>
       <c r="B33">
         <v>5.9800838574423497E-2</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>2.8276712635945701E-2</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="B35">
         <v>0.28434566156839203</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>4.6488644808461599E-2</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="B37">
         <v>8.6518725068742502E-2</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="38" spans="1:25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>19</v>
       </c>
       <c r="B38">
         <v>0.15342728502474001</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="39" spans="1:25">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="B39">
         <v>0.52726763090032502</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
       <c r="B40">
         <v>-2.6530575436901498E-2</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="41" spans="1:25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="B41">
         <v>4.9423393739703499E-3</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>0.57033876959477503</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>24</v>
       </c>
       <c r="B43">
         <v>0.285993108026383</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="B44">
         <v>8.1768877763871498E-2</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="B45">
         <v>3.6333841894106302E-2</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="46" spans="1:25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
       <c r="B46">
         <v>4.2553191489361701E-2</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B47">
         <v>3.9215686274509803E-2</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="B48">
         <v>-2.8818443804034602E-3</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="49" spans="1:25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="B49">
         <v>4.9423393739703499E-3</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="50" spans="1:25">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>31</v>
       </c>
       <c r="B50">
         <v>-5.0829542761900701E-2</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="51" spans="1:25">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="B51">
         <v>6.5428764520142199E-3</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="52" spans="1:25">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B52">
         <v>1.00908173562059E-3</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="53" spans="1:25">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B53">
         <v>-0.387382150686086</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="54" spans="1:25">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="B54">
         <v>1.00908173562059E-3</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="55" spans="1:25">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B55">
         <v>-7.0999529876991499E-2</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="B56">
         <v>2.2222222222222199E-2</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="57" spans="1:25">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="B57">
         <v>2.32558139534884E-2</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="58" spans="1:25">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>39</v>
       </c>
       <c r="B58">
         <v>7.9282150236163695E-2</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="59" spans="1:25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="B59">
         <v>0.10914070605959</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="60" spans="1:25">
       <c r="A60" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="B60">
         <v>2.8818443804034602E-3</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="B61">
         <v>2.63757873996311E-2</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="62" spans="1:25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B62">
         <v>2.3173768489352601E-2</v>
@@ -2509,7 +2509,7 @@
     </row>
     <row r="63" spans="1:25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>44</v>
       </c>
       <c r="B63">
         <v>0.33083430637685401</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="64" spans="1:25">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="B64">
         <v>6.6908559955997399E-2</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="65" spans="1:25">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="B65">
         <v>0.28105076865241202</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="66" spans="1:25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>47</v>
       </c>
       <c r="B66">
         <v>-0.57033876959477503</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
       <c r="B67">
         <v>4.9423393739703499E-3</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="68" spans="1:25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="B68">
         <v>-0.57033876959477503</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="69" spans="1:25">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="B69">
         <v>0.14332690177620999</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="70" spans="1:25">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>51</v>
       </c>
       <c r="B70">
         <v>6.4775413711583907E-2</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="71" spans="1:25">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="B71">
         <v>3.7187359592631399E-2</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="72" spans="1:25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="B72">
         <v>1.7094017094017099E-2</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="73" spans="1:25">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="B73">
         <v>0.242981533096398</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="74" spans="1:25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>55</v>
       </c>
       <c r="B74">
         <v>-5.9800838574423497E-2</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="75" spans="1:25">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>56</v>
       </c>
       <c r="B75">
         <v>3.2948929159802298E-3</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c r="B76">
         <v>-1.6474464579901199E-3</v>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="77" spans="1:25">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>58</v>
       </c>
       <c r="B77">
         <v>1.5533980582524301E-2</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="78" spans="1:25">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B78">
         <v>4.3810693218469997E-2</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="79" spans="1:25">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B79">
         <v>0.50073705546342395</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="80" spans="1:25">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B80">
         <v>-7.3705546342362296E-4</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="81" spans="1:25">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="B81">
         <v>1.6474464579901199E-3</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="82" spans="1:25">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="B82">
         <v>7.2339181286549703E-2</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="83" spans="1:25">
       <c r="A83" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="B83">
         <v>1.6474464579901199E-3</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="84" spans="1:25">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="B84">
         <v>1.6474464579901199E-3</v>
@@ -3093,7 +3093,7 @@
     </row>
     <row r="85" spans="1:25">
       <c r="A85" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B85">
         <v>0.28434566156839203</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="C86">
         <v>7.2046109510086498E-2</v>
@@ -3243,7 +3243,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="A3:A1048576"/>
   </sortState>
@@ -3261,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="AB29" sqref="AB29"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="13"/>
@@ -3272,10 +3271,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -3349,10 +3348,11 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B2">
-        <v>-6.4427271428077498E-2</v>
+        <f>COUNT(C2:Y2)</f>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>-5.7636887608069204E-3</v>
@@ -3372,10 +3372,11 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="B3">
-        <v>-1.3245033112582801E-2</v>
+        <f t="shared" ref="B3:B66" si="0">COUNT(C3:Y3)</f>
+        <v>1</v>
       </c>
       <c r="X3">
         <v>-1.3245033112582801E-2</v>
@@ -3383,10 +3384,11 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B4">
-        <v>-1.7094017094017099E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>-1.7094017094017099E-2</v>
@@ -3394,10 +3396,11 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="B5">
-        <v>7.5519581876348002E-3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2.8818443804034602E-3</v>
@@ -3414,10 +3417,11 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="B6">
-        <v>7.5519581876348002E-3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>2.8818443804034602E-3</v>
@@ -3434,10 +3438,11 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="B7">
-        <v>-1.7094017094017099E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>-1.7094017094017099E-2</v>
@@ -3445,10 +3450,11 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B8">
-        <v>3.7187359592631399E-2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>3.6363636363636397E-2</v>
@@ -3459,10 +3465,11 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B9">
-        <v>7.3705546342362296E-4</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="P9">
         <v>7.3705546342362296E-4</v>
@@ -3470,10 +3477,11 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B10">
-        <v>-2.92397660818713E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>-2.92397660818713E-3</v>
@@ -3481,10 +3489,11 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="B11">
-        <v>-5.1182238315494802E-2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>-5.7636887608069204E-3</v>
@@ -3501,10 +3510,11 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="B12">
-        <v>0.26919513080620899</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>7.2046109510086496E-3</v>
@@ -3542,10 +3552,11 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B13">
-        <v>-1.0202927404832401E-2</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>-1.4409221902017301E-3</v>
@@ -3580,10 +3591,11 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B14">
-        <v>-2.3225878898450801E-3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="J14">
         <v>-1.7391304347826101E-2</v>
@@ -3600,10 +3612,11 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B15">
-        <v>7.5519581876348002E-3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>2.8818443804034602E-3</v>
@@ -3620,10 +3633,11 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="B16">
-        <v>5.2751574799262201E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H16">
         <v>1.7094017094017099E-2</v>
@@ -3643,10 +3657,11 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
         <v>11</v>
-      </c>
-      <c r="B17">
-        <v>-0.387382150686086</v>
       </c>
       <c r="D17">
         <v>-4.4444444444444398E-2</v>
@@ -3684,10 +3699,11 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="B18">
-        <v>0.57033876959477503</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>1.1527377521613799E-2</v>
@@ -3755,10 +3771,11 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B19">
-        <v>-5.1182238315494802E-2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>-5.7636887608069204E-3</v>
@@ -3775,10 +3792,11 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="B20">
-        <v>1.7094017094017099E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1.7094017094017099E-2</v>
@@ -3786,10 +3804,11 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="B21">
-        <v>1.3245033112582801E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="X21">
         <v>1.3245033112582801E-2</v>
@@ -3797,10 +3816,11 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="B22">
-        <v>2.92397660818713E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="O22">
         <v>2.92397660818713E-3</v>
@@ -3808,10 +3828,11 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="B23">
-        <v>2.3225878898450801E-3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="J23">
         <v>1.7391304347826101E-2</v>
@@ -3828,10 +3849,11 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="B24">
-        <v>5.1182238315494802E-2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>5.7636887608069204E-3</v>
@@ -3848,10 +3870,11 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="B25">
-        <v>6.6908559955997399E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>8.6455331412103806E-3</v>
@@ -3871,10 +3894,11 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="B26">
-        <v>-0.285993108026383</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>-5.7636887608069204E-3</v>
@@ -3945,10 +3969,11 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B27">
-        <v>2.8818443804034602E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>2.8818443804034602E-3</v>
@@ -3956,10 +3981,11 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B28">
-        <v>0.59935063355959595</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>1.4409221902017299E-2</v>
@@ -4021,10 +4047,11 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B29">
-        <v>5.0829542761900701E-2</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="O29">
         <v>5.8479532163742704E-3</v>
@@ -4047,10 +4074,11 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B30">
-        <v>0.387382150686086</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>4.4444444444444398E-2</v>
@@ -4088,10 +4116,11 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B31">
-        <v>-2.8818443804034602E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>-2.8818443804034602E-3</v>
@@ -4099,10 +4128,11 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B32">
-        <v>-2.63757873996311E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H32">
         <v>-8.5470085470085496E-3</v>
@@ -4122,10 +4152,11 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B33">
-        <v>5.9800838574423497E-2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="G33">
         <v>2.5000000000000001E-2</v>
@@ -4139,10 +4170,11 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B34">
-        <v>2.8276712635945701E-2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R34">
         <v>6.0544904137235104E-3</v>
@@ -4153,10 +4185,11 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="B35">
-        <v>0.28434566156839203</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>5.7636887608069204E-3</v>
@@ -4227,10 +4260,11 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>4.6488644808461599E-2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="P36">
         <v>6.4492353049566999E-3</v>
@@ -4244,10 +4278,11 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B37">
-        <v>8.6518725068742502E-2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I37">
         <v>4.6783625730994198E-2</v>
@@ -4258,10 +4293,11 @@
     </row>
     <row r="38" spans="1:25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B38">
-        <v>0.15342728502474001</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>8.6455331412103806E-3</v>
@@ -4284,10 +4320,11 @@
     </row>
     <row r="39" spans="1:25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B39">
-        <v>0.52726763090032502</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E39">
         <v>0.5</v>
@@ -4301,10 +4338,11 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
       <c r="B40">
-        <v>-2.6530575436901498E-2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="P40">
         <v>7.3705546342362296E-4</v>
@@ -4318,10 +4356,11 @@
     </row>
     <row r="41" spans="1:25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="B41">
-        <v>4.9423393739703499E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="Y41">
         <v>4.9423393739703499E-3</v>
@@ -4329,10 +4368,11 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>23</v>
       </c>
       <c r="B42">
-        <v>0.57033876959477503</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="C42">
         <v>1.1527377521613799E-2</v>
@@ -4400,10 +4440,11 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B43">
-        <v>0.285993108026383</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="C43">
         <v>5.7636887608069204E-3</v>
@@ -4474,10 +4515,11 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="B44">
-        <v>8.1768877763871498E-2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="Q44">
         <v>3.9215686274509803E-2</v>
@@ -4488,10 +4530,11 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="B45">
-        <v>3.6333841894106302E-2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C45">
         <v>-2.8818443804034602E-3</v>
@@ -4502,10 +4545,11 @@
     </row>
     <row r="46" spans="1:25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
       <c r="B46">
-        <v>4.2553191489361701E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="S46">
         <v>4.2553191489361701E-2</v>
@@ -4513,10 +4557,11 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B47">
-        <v>3.9215686274509803E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="Q47">
         <v>3.9215686274509803E-2</v>
@@ -4524,10 +4569,11 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B48">
-        <v>-2.8818443804034602E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C48">
         <v>-2.8818443804034602E-3</v>
@@ -4535,10 +4581,11 @@
     </row>
     <row r="49" spans="1:25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="B49">
-        <v>4.9423393739703499E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="Y49">
         <v>4.9423393739703499E-3</v>
@@ -4546,10 +4593,11 @@
     </row>
     <row r="50" spans="1:25">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B50">
-        <v>-5.0829542761900701E-2</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="O50">
         <v>-5.8479532163742704E-3</v>
@@ -4572,10 +4620,11 @@
     </row>
     <row r="51" spans="1:25">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="B51">
-        <v>6.5428764520142199E-3</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>2.8818443804034602E-3</v>
@@ -4589,10 +4638,11 @@
     </row>
     <row r="52" spans="1:25">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B52">
-        <v>1.00908173562059E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="R52">
         <v>1.00908173562059E-3</v>
@@ -4600,10 +4650,11 @@
     </row>
     <row r="53" spans="1:25">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B53">
-        <v>-0.387382150686086</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>-4.4444444444444398E-2</v>
@@ -4641,10 +4692,11 @@
     </row>
     <row r="54" spans="1:25">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="B54">
-        <v>1.00908173562059E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="R54">
         <v>1.00908173562059E-3</v>
@@ -4652,10 +4704,11 @@
     </row>
     <row r="55" spans="1:25">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B55">
-        <v>-7.0999529876991499E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>-2.2222222222222199E-2</v>
@@ -4675,10 +4728,11 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="B56">
-        <v>2.2222222222222199E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>2.2222222222222199E-2</v>
@@ -4686,10 +4740,11 @@
     </row>
     <row r="57" spans="1:25">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="B57">
-        <v>2.32558139534884E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="V57">
         <v>2.32558139534884E-2</v>
@@ -4697,10 +4752,11 @@
     </row>
     <row r="58" spans="1:25">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B58">
-        <v>7.9282150236163695E-2</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="H58">
         <v>1.7094017094017099E-2</v>
@@ -4726,10 +4782,11 @@
     </row>
     <row r="59" spans="1:25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="B59">
-        <v>0.10914070605959</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="N59">
         <v>5.3333333333333302E-2</v>
@@ -4749,10 +4806,11 @@
     </row>
     <row r="60" spans="1:25">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="B60">
-        <v>2.8818443804034602E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>2.8818443804034602E-3</v>
@@ -4760,10 +4818,11 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="B61">
-        <v>2.63757873996311E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H61">
         <v>8.5470085470085496E-3</v>
@@ -4783,10 +4842,11 @@
     </row>
     <row r="62" spans="1:25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B62">
-        <v>2.3173768489352601E-2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J62">
         <v>1.7391304347826101E-2</v>
@@ -4800,10 +4860,11 @@
     </row>
     <row r="63" spans="1:25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>44</v>
       </c>
       <c r="B63">
-        <v>0.33083430637685401</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="C63">
         <v>5.7636887608069204E-3</v>
@@ -4871,10 +4932,11 @@
     </row>
     <row r="64" spans="1:25">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="B64">
-        <v>6.6908559955997399E-2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>8.6455331412103806E-3</v>
@@ -4894,10 +4956,11 @@
     </row>
     <row r="65" spans="1:25">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="B65">
-        <v>0.28105076865241202</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="C65">
         <v>5.7636887608069204E-3</v>
@@ -4968,10 +5031,11 @@
     </row>
     <row r="66" spans="1:25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>47</v>
       </c>
       <c r="B66">
-        <v>-0.57033876959477503</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="C66">
         <v>-1.1527377521613799E-2</v>
@@ -5039,10 +5103,11 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
       <c r="B67">
-        <v>4.9423393739703499E-3</v>
+        <f t="shared" ref="B67:B86" si="1">COUNT(C67:Y67)</f>
+        <v>1</v>
       </c>
       <c r="Y67">
         <v>4.9423393739703499E-3</v>
@@ -5050,10 +5115,11 @@
     </row>
     <row r="68" spans="1:25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="B68">
-        <v>-0.57033876959477503</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="C68">
         <v>-1.1527377521613799E-2</v>
@@ -5121,10 +5187,11 @@
     </row>
     <row r="69" spans="1:25">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="B69">
-        <v>0.14332690177620999</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="C69">
         <v>2.8818443804034602E-3</v>
@@ -5150,10 +5217,11 @@
     </row>
     <row r="70" spans="1:25">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>51</v>
       </c>
       <c r="B70">
-        <v>6.4775413711583907E-2</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="D70">
         <v>2.2222222222222199E-2</v>
@@ -5164,10 +5232,11 @@
     </row>
     <row r="71" spans="1:25">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="B71">
-        <v>3.7187359592631399E-2</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="F71">
         <v>3.6363636363636397E-2</v>
@@ -5178,10 +5247,11 @@
     </row>
     <row r="72" spans="1:25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="B72">
-        <v>1.7094017094017099E-2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>1.7094017094017099E-2</v>
@@ -5189,10 +5259,11 @@
     </row>
     <row r="73" spans="1:25">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="B73">
-        <v>0.242981533096398</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="C73">
         <v>2.8818443804034602E-3</v>
@@ -5245,10 +5316,11 @@
     </row>
     <row r="74" spans="1:25">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="B74">
-        <v>-5.9800838574423497E-2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="G74">
         <v>-2.5000000000000001E-2</v>
@@ -5262,10 +5334,11 @@
     </row>
     <row r="75" spans="1:25">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>56</v>
       </c>
       <c r="B75">
-        <v>3.2948929159802298E-3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Y75">
         <v>3.2948929159802298E-3</v>
@@ -5273,10 +5346,11 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c r="B76">
-        <v>-1.6474464579901199E-3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Y76">
         <v>-1.6474464579901199E-3</v>
@@ -5284,10 +5358,11 @@
     </row>
     <row r="77" spans="1:25">
       <c r="A77" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B77">
-        <v>1.5533980582524301E-2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K77">
         <v>1.5533980582524301E-2</v>
@@ -5295,10 +5370,11 @@
     </row>
     <row r="78" spans="1:25">
       <c r="A78" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="B78">
-        <v>4.3810693218469997E-2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="K78">
         <v>1.5533980582524301E-2</v>
@@ -5312,10 +5388,11 @@
     </row>
     <row r="79" spans="1:25">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B79">
-        <v>0.50073705546342395</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="E79">
         <v>0.5</v>
@@ -5326,10 +5403,11 @@
     </row>
     <row r="80" spans="1:25">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B80">
-        <v>-7.3705546342362296E-4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="P80">
         <v>-7.3705546342362296E-4</v>
@@ -5337,10 +5415,11 @@
     </row>
     <row r="81" spans="1:25">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="B81">
-        <v>1.6474464579901199E-3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Y81">
         <v>1.6474464579901199E-3</v>
@@ -5348,10 +5427,11 @@
     </row>
     <row r="82" spans="1:25">
       <c r="A82" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B82">
-        <v>7.2339181286549703E-2</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="N82">
         <v>5.3333333333333302E-2</v>
@@ -5362,10 +5442,11 @@
     </row>
     <row r="83" spans="1:25">
       <c r="A83" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="B83">
-        <v>1.6474464579901199E-3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Y83">
         <v>1.6474464579901199E-3</v>
@@ -5373,10 +5454,11 @@
     </row>
     <row r="84" spans="1:25">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="B84">
-        <v>1.6474464579901199E-3</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Y84">
         <v>1.6474464579901199E-3</v>
@@ -5384,10 +5466,11 @@
     </row>
     <row r="85" spans="1:25">
       <c r="A85" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B85">
-        <v>0.28434566156839203</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="C85">
         <v>5.7636887608069204E-3</v>
@@ -5458,83 +5541,102 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" t="s">
-        <v>35</v>
-      </c>
-      <c r="B86" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C86">
-        <v>7.2046109510086498E-2</v>
+        <f>COUNT(C2:C85)</f>
+        <v>31</v>
       </c>
       <c r="D86">
-        <v>0.155555555555556</v>
+        <f t="shared" ref="D86:Y86" si="2">COUNT(D2:D85)</f>
+        <v>18</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="F86">
-        <v>0.2</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="G86">
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="H86">
-        <v>0.230769230769231</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="I86">
-        <v>0.11111111111111099</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="J86">
-        <v>5.21739130434783E-2</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="K86">
-        <v>4.8543689320388397E-2</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="L86">
-        <v>0.162790697674419</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="M86">
-        <v>0.19148936170212799</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="N86">
-        <v>0.146666666666667</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="O86">
-        <v>0.105263157894737</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="P86">
-        <v>3.4457342915054402E-2</v>
+        <f t="shared" si="2"/>
+        <v>32</v>
       </c>
       <c r="Q86">
-        <v>0.21568627450980399</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="R86">
-        <v>5.9535822401614598E-2</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="S86">
-        <v>0.19148936170212799</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="T86">
-        <v>0.113207547169811</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="U86">
-        <v>0.17647058823529399</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="V86">
-        <v>0.162790697674419</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="W86">
-        <v>0.24444444444444399</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="X86">
-        <v>0.139072847682119</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="Y86">
-        <v>7.0840197693574997E-2</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5557,196 +5659,194 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A1:XFD1048576">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Cleaned up core model
</commit_message>
<xml_diff>
--- a/data/minspan_EcoliCore.xlsx
+++ b/data/minspan_EcoliCore.xlsx
@@ -3260,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="13"/>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86">
         <f>COUNT(C2:C85)</f>

</xml_diff>